<commit_message>
Added ability to specify nearby location type; fixed some bugs! :)
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory.Console/Scenes.xlsx
+++ b/Solution/NeverendingStory.Console/Scenes.xlsx
@@ -60,7 +60,7 @@
     <t xml:space="preserve">Go to work like always and see if anything changes</t>
   </si>
   <si>
-    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:fortress:namewiththe:baronhome}. You know the way, which leads through the nearby {location:nearby:name:pathtobaron}.{|GOTO:pathtobaron|}{|SET:goal:baronhome|}
+    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:fortress:namewiththe:baronhome}. You know the way, which leads through the nearby {location:nearby:forest|swamp:pathtobaron:name}.{|GOTO:pathtobaron|}{|SET:goal:baronhome|}
 Deep in {location:current:namewiththe}, a {character:mentor:sexAge:ranger} emerges from behind the {location:current:covers}. {character:mentor:subPronoun:cap}'s wearing rough clothing.{|MTM|}</t>
   </si>
   <si>
@@ -91,8 +91,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">You slink into the nearby {location:nearby:name:pathtobaron} in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}
-The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the </t>
+      <t xml:space="preserve">You slink into the nearby {location:nearby:</t>
     </r>
     <r>
       <rPr>
@@ -100,7 +99,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{location:current:covers}</t>
+      <t xml:space="preserve">forest|swamp</t>
     </r>
     <r>
       <rPr>
@@ -109,7 +108,25 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
+      <t xml:space="preserve">:pathtobaron:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">} in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}
+The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the {location:current:covers}. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
     </r>
   </si>
   <si>
@@ -121,8 +138,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">You find a group of the {character:baron:baron}'s men in the tavern drinking. As one of them turns to you, your first blow lands squarely on his jaw. An all-out brawl breaks out. You give as good as you get, but in the end there are too many of them.
-"I'll take care of {objPronoun}," you hear a voice say. Rough hands carry you out of town into the nearby {location:nearby:name:pathtobaron}. You pass out.{|GOTO:pathtobaron|}
-You wake up the next day, deep in {location:current:namewiththe}. A {character:mentor:sexAge:ranger} sits under a nearby </t>
+"I'll take care of {objPronoun}," you hear a voice say. Rough hands carry you out of town into the nearby {location:nearby:</t>
     </r>
     <r>
       <rPr>
@@ -130,7 +146,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{location:current:cover}</t>
+      <t xml:space="preserve">forest|swamp</t>
     </r>
     <r>
       <rPr>
@@ -139,111 +155,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">MTM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goal:baronhome&amp;character:ranger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"My name's {character:ranger:name}," {character:ranger:subPronoun} says. "{location:hometown:name}'s not the first village that {character:baron:baron} {character:baron:name}'s taken control of. {character:baron:subPronoun:cap}'ll stop at nothing until the whole region is under {character:baron:possPronoun} control. We can't let that happen.
-"If you want to stop {character:baron:objPronoun} and get back {location:hometown:name}, you'll have to make it to {location:baronhome:namewiththe}."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ask {character:ranger:name} for {character:ranger:possPronoun} help</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set off for {location:baronhome:namewiththe} (you know the way)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"I'm sorry, I can't go near the {character:baron:baron}'s {location:baronhome:type:cap} myself. {character:baron:subPronoun:cap} and {character:baron:possPronoun} goons'll be looking for me. But here, you take this." {character:ranger:subPronoun:cap} hands you piece of rolled cloth. "It might be useful." With that, {character:ranger:name} disappears into the {location:current:type}. {|GIVE:map:A cloth map:shows a hidden path into [location-baronhome-namewiththe]|}
-The cloth, once unrolled, looks like some sort of map of a secret entrance into the {character:baron:baron}'s {location:baronhome:type:cap}. You roll it up again and put it in your pack.
-You travel through {location:current:namewiththe} for several days.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You walk further into the {location:current:type}, headed for {location:goal:namewiththe}. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
-You travel through {location:current:namewiththe} for several days.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location:current:forest|location:current:mountain|location:current:plains</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A wide river blocks your path to {location:goal:namewiththe}. The water is deep and moving fast.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wade through the rushing water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Look for another way around</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You wade through the rushing water. It comes up to your armpits. You hold your pack above your head.
-It takes every ounce of your strength, but you make it across. On the other side, you're soaked to the bone and exhausted. You rest for an hour while your clothes dry.
-Once you're ready, you continue on your way to {location:goal:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You walk along the river's edge until you find an enormous tree trunk lying across the river. It looks as though someone has recently cut it down. You're able to nimbly walk across the log and cross the river.
-On the other side, you continue on your way to {location:goal:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location:current:forest|location:current:plains</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A long, tall wall runs across your path to {location:goal:namewiththe}, at least 15 feet tall. Its stones are old and falling apart, but it might collapse on top of you if you try to climb it.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Climb the wall here</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Looking for a gap in the wall somewhere else</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You pull stones out of the wall as you climb, and they clatter to the ground below you. The wall shifts and sways as you climb, but miraculously doesn't collapse. When you get to the top and descend on the other side, you can hear stones skidding out of place behind you.
-You continue on your way to {location:goal:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Further along the wall, you find a tall tree with a branch leaning over the wall. You climb the tree, edge out along the branch, and drop down on the other side of the wall.
-Once over the wall, you continue on your way to {location:goal:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOTW1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:forest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your path lies through a thick {location:current:type}, overgrown and difficult to travel through.
-After a day or so, you hear footsteps crashing through the brush. They're getting nearer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hide in the brush and wait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seek out the footsteps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You find a clump of bushes to hide inside. As the footsteps get closer, you see two dozen of the {character:baron:baron}'s armed men tramping through the underbrush.
-You hold your breath, but one of them stumbles just too close to you.
-"What do we have here?" he says. He grabs you roughly by the shoulder and jerks you to your feet. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">You tramp through the underbrush towards the sound of footsteps, getting closer as you hike. Then, through the </t>
+      <t xml:space="preserve">:pathtobaron:</t>
     </r>
     <r>
       <rPr>
@@ -251,7 +163,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{location:current:covers}</t>
+      <t xml:space="preserve">name</t>
     </r>
     <r>
       <rPr>
@@ -260,9 +172,106 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">, two dozen of the {character:baron:baron}'s men in uniform emerge.
+      <t xml:space="preserve">}. You pass out.{|GOTO:pathtobaron|}
+You wake up the next day, deep in {location:current:namewiththe}. A {character:mentor:sexAge:ranger} sits under a nearby {location:current:cover}. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">MTM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal:baronhome&amp;character:ranger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"My name's {character:ranger:name}," {character:ranger:subPronoun} says. "{location:hometown:name}'s not the first village that {character:baron:baron} {character:baron:name}'s taken control of. {character:baron:subPronoun:cap}'ll stop at nothing until the whole region is under {character:baron:possPronoun} control. We can't let that happen.
+"If you want to stop {character:baron:objPronoun} and get back {location:hometown:name}, you'll have to make it to {location:baronhome:namewiththe}."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ask {character:ranger:name} for {character:ranger:possPronoun} help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set off for {location:baronhome:namewiththe} (you know the way)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"I'm sorry, I can't go near the {character:baron:baron}'s {location:baronhome:type:cap} myself. {character:baron:subPronoun:cap} and {character:baron:possPronoun} goons'll be looking for me. But here, you take this." {character:ranger:subPronoun:cap} hands you piece of rolled cloth. "It might be useful." With that, {character:ranger:name} disappears into the {location:current:type}. {|GIVE:map:A cloth map:shows a hidden path into [location-baronhome-namewiththe]|}
+The cloth, once unrolled, looks like some sort of map of a secret entrance into the {character:baron:baron}'s {location:baronhome:type:cap}. You roll it up again and put it in your pack.
+You travel through {location:current:namewiththe} for several days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You walk further into the {location:current:type}, headed for {location:goal:namewiththe}. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
+You travel through {location:current:namewiththe} for several days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location:current:forest|location:current:mountain|location:current:plains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A wide river blocks your path to {location:goal:namewiththe}. The water is deep and moving fast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wade through the rushing water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look for another way around</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You wade through the rushing water. It comes up to your armpits. You hold your pack above your head.
+It takes every ounce of your strength, but you make it across. On the other side, you're soaked to the bone and exhausted. You rest for an hour while your clothes dry.
+Once you're ready, you continue on your way to {location:goal:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You walk along the river's edge until you find an enormous tree trunk lying across the river. It looks as though someone has recently cut it down. You're able to nimbly walk across the log and cross the river.
+On the other side, you continue on your way to {location:goal:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location:current:forest|location:current:plains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A long, tall wall runs across your path to {location:goal:namewiththe}, at least 15 feet tall. Its stones are old and falling apart, but it might collapse on top of you if you try to climb it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Climb the wall here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking for a gap in the wall somewhere else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You pull stones out of the wall as you climb, and they clatter to the ground below you. The wall shifts and sways as you climb, but miraculously doesn't collapse. When you get to the top and descend on the other side, you can hear stones skidding out of place behind you.
+You continue on your way to {location:goal:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further along the wall, you find a tall tree with a branch leaning over the wall. You climb the tree, edge out along the branch, and drop down on the other side of the wall.
+Once over the wall, you continue on your way to {location:goal:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOTW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your path lies through a thick {location:current:type}, overgrown and difficult to travel through.
+After a day or so, you hear footsteps crashing through the brush. They're getting nearer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide in the brush and wait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seek out the footsteps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You find a clump of bushes to hide inside. As the footsteps get closer, you see two dozen of the {character:baron:baron}'s armed men tramping through the underbrush.
+You hold your breath, but one of them stumbles just too close to you.
+"What do we have here?" he says. He grabs you roughly by the shoulder and jerks you to your feet. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You tramp through the underbrush towards the sound of footsteps, getting closer as you hike. Then, through the {location:current:covers}, two dozen of the {character:baron:baron}'s men in uniform emerge.
 One of them grabs you roughly by the shoulder. "What do we have here?" he says. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">BOTW1a</t>
@@ -549,46 +558,14 @@
     <t xml:space="preserve">chasedbybaron:true</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">{|GOTO:hometown|}You finally return to {location:current:name}. The people have been under the rule of the {character:baron:baron}'s men since you left, who have done nothing but drink and destroy property that isn't theirs. The men pursuing you are close behind, maybe a day or so.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">{|MOTW1|}</t>
-    </r>
+    <t xml:space="preserve">{|GOTO:hometown|}You finally return to {location:current:name}. The people have been under the rule of the {character:baron:baron}'s men since you left, who have done nothing but drink and destroy property that isn't theirs. The men pursuing you are close behind, maybe a day or so.{|MOTW1|}</t>
   </si>
   <si>
     <t xml:space="preserve">MOTW1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">You organize a secret meeting at night to rally the people together. You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:current:namewiththe}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they retreat, leaving the town forever.
-The next day, the men who were pursuing you arrive. {location:current:namewiththe:cap}'s finest easily chases them off. There is strength in numbers, and they knew what to expect, thanks to you.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">{|FTL1|}</t>
-    </r>
+    <t xml:space="preserve">You organize a secret meeting at night to rally the people together. You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:current:namewiththe}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they retreat, leaving the town forever.
+The next day, the men who were pursuing you arrive. {location:current:namewiththe:cap}'s finest easily chases them off. There is strength in numbers, and they knew what to expect, thanks to you.{|FTL1|}</t>
   </si>
   <si>
     <t xml:space="preserve">FTL1</t>
@@ -995,11 +972,11 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="64.82"/>

</xml_diff>

<commit_message>
Fixing "Chief" bug; adding horrible almanac
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory.Console/Scenes.xlsx
+++ b/Solution/NeverendingStory.Console/Scenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="159">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -60,7 +60,7 @@
     <t xml:space="preserve">Go to work like always and see if anything changes</t>
   </si>
   <si>
-    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:fortress:namewiththe:baronhome}. You know the way, which leads through the nearby {location:nearby:forest|swamp:pathtobaron:name}.{|GOTO:pathtobaron|}{|SET:goal:baronhome|}
+    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:fortress:namewiththe:baronhome}. You know the way, which leads through the nearby {location:nearby:forest|mountain|swamp|plains:pathtobaron:name}.{|GOTO:pathtobaron|}{|SET:goal:baronhome|}
 Deep in {location:current:namewiththe}, a {character:mentor:sexAge:ranger} emerges from behind the {location:current:covers}. {character:mentor:subPronoun:cap}'s wearing rough clothing.{|MTM|}</t>
   </si>
   <si>
@@ -99,7 +99,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">forest|swamp</t>
+      <t xml:space="preserve">forest|mountain|swamp|plains</t>
     </r>
     <r>
       <rPr>
@@ -108,24 +108,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">:pathtobaron:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">} in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}
+      <t xml:space="preserve">:pathtobaron:name} in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}
 The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the {location:current:covers}. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
     </r>
   </si>
@@ -146,7 +129,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">forest|swamp</t>
+      <t xml:space="preserve">forest|mountain|swamp|plains</t>
     </r>
     <r>
       <rPr>
@@ -155,24 +138,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">:pathtobaron:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}. You pass out.{|GOTO:pathtobaron|}
+      <t xml:space="preserve">:pathtobaron:name}. You pass out.{|GOTO:pathtobaron|}
 You wake up the next day, deep in {location:current:namewiththe}. A {character:mentor:sexAge:ranger} sits under a nearby {location:current:cover}. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?"</t>
     </r>
   </si>
@@ -202,10 +168,10 @@
 You travel through {location:current:namewiththe} for several days.</t>
   </si>
   <si>
-    <t xml:space="preserve">CTT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location:current:forest|location:current:mountain|location:current:plains</t>
+    <t xml:space="preserve">CTT1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location:current:forest</t>
   </si>
   <si>
     <t xml:space="preserve">A wide river blocks your path to {location:goal:namewiththe}. The water is deep and moving fast.</t>
@@ -226,10 +192,42 @@
 On the other side, you continue on your way to {location:goal:namewiththe}.</t>
   </si>
   <si>
-    <t xml:space="preserve">CTT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location:current:forest|location:current:plains</t>
+    <t xml:space="preserve">CTT1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location:current:plains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You walk along the river's edge until you find a number of long wooden planks lying across the river. You wonder who put them there. You're able to walk carefully across the planks and cross the river.
+On the other side, you continue on your way to {location:goal:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTT1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location:current:mountain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A fast-rushing river blocks your path to {location:goal:namewiththe}. The water is deep and moving fast. You can see stepping stones barely visible under the surface of the water.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross on the stepping stones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look for a better place to cross farther up</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> You step very carefully on each stone. Planting your feet solidly on each stone before stepping to the next one, you make it about halfway across the river. Suddenly, a stone that you were stepping on comes loose, careening down the raging river and taking you along with it.
+You get several bruises before you’re able to catch yourself, much further downstream, including a nasty bruise on your head. You drag yourself to the other side of the river. You’re sore all over, and can’t move for hours.
+Once you feel almost ready, you climb back up the river’s edge to the path and continue on your way to {location:goal:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You climb up the rocks along the river's edge until you find an enormous tree trunk lying across the river. It looks as though someone has recently cut it down. You're able to nimbly walk across the log and cross the river.
+Climbing back down, you find the path again and continue on your way to
+ {location:goal:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTT2.1</t>
   </si>
   <si>
     <t xml:space="preserve">A long, tall wall runs across your path to {location:goal:namewiththe}, at least 15 feet tall. Its stones are old and falling apart, but it might collapse on top of you if you try to climb it.</t>
@@ -238,7 +236,7 @@
     <t xml:space="preserve">Climb the wall here</t>
   </si>
   <si>
-    <t xml:space="preserve">Looking for a gap in the wall somewhere else</t>
+    <t xml:space="preserve">Look for a gap in the wall somewhere else</t>
   </si>
   <si>
     <t xml:space="preserve">You pull stones out of the wall as you climb, and they clatter to the ground below you. The wall shifts and sways as you climb, but miraculously doesn't collapse. When you get to the top and descend on the other side, you can hear stones skidding out of place behind you.
@@ -249,13 +247,30 @@
 Once over the wall, you continue on your way to {location:goal:namewiththe}.</t>
   </si>
   <si>
+    <t xml:space="preserve">CTT2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location:current:swamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A long, tall wall runs across your path to {location:goal:namewiththe}, still standing despite the base of it being buried in muck. Its stones are old and falling apart, but it might collapse on top of you if you try to climb it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You pull stones out of the wall as you climb, and they clatter into the muck beneath you. The wall shifts and sways as you climb, but miraculously doesn't collapse. When you get to the top and descend on the other side, you can hear stones skidding out of place behind you and plopping into the {location:current:type}, never to be seen again.
+You continue on your way to {location:goal:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farther along the wall, you find a number of thick vines that have grown up over the stones here. You take hold of the vines, pulling yourself carefully to the top, before letting yourself down the other side. Your feet squelch when they hit the {location:current:type}.
+You continue on your way to {location:goal:namewiththe}.</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOTW1</t>
   </si>
   <si>
     <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:forest</t>
   </si>
   <si>
-    <t xml:space="preserve">Your path lies through a thick {location:current:type}, overgrown and difficult to travel through.
+    <t xml:space="preserve">The {location:current:type} is dense here, overgrown and difficult to travel through.
 After a day or so, you hear footsteps crashing through the brush. They're getting nearer.</t>
   </si>
   <si>
@@ -296,10 +311,7 @@
 You travel for a few minutes away from the camp before you realize {character:ranger:name} is gone. The sun begins to rise as you silently make your way toward {location:goal:namewiththe}.</t>
   </si>
   <si>
-    <t xml:space="preserve">BOTW2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">location:current:forest|location:current:mountain</t>
+    <t xml:space="preserve">BOTW2.1</t>
   </si>
   <si>
     <t xml:space="preserve">Your path lies through a thick {location:current:type}, overgrown and difficult to travel through.
@@ -321,7 +333,18 @@
     <t xml:space="preserve">It seems like it takes an eternity, but eventually, as it’s getting dark outside again, the two bears settle down, nestled up against each other. You wait until you’re absolutely sure they’re asleep. Then, very, very quietly, you gather your bedroll and sneak past them out of the cave. The rain has stopped by now, and the {location:current:type} is quiet and dark.</t>
   </si>
   <si>
+    <t xml:space="preserve">BOTW2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The mountain pass is rough here. In many places, you have to climb on all fours to make it over the enormous, jagged rocks.
+After a day or so, it begins to rain heavily. You take shelter in a nearby cave, making your bed in a small alcove. You go to sleep to wait out the rain.
+When you wake up, you hear someone else moving in the cave. Opening your eyes, you see two enormous bears, sitting between your alcove and the door. It’s still raining outside. They seem to be getting ready to lie down. What do you do?</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location:current:forest|location:current:mountain</t>
   </si>
   <si>
     <t xml:space="preserve">The next day, a small creature runs across your path. You almost step on it.
@@ -355,7 +378,7 @@
     <t xml:space="preserve">Wait until {character:petowner:subPronoun}'s gone and continue</t>
   </si>
   <si>
-    <t xml:space="preserve">You step out from hiding, startling the {character:petowner:sexAge} briefly. {character:petowner:subPronoun:cap} seems thrilled to have the help. {character:petowner:subPronoun:cap} tells you {character:petowner:possPronoun} name is {character:petowner:name}, and {character:petowner:possPronoun} cat's name is Sniffles.
+    <t xml:space="preserve">You step out of hiding, startling the {character:petowner:sexAge} briefly. {character:petowner:subPronoun:cap} seems thrilled to have the help. {character:petowner:subPronoun:cap} tells you {character:petowner:possPronoun} name is {character:petowner:name}, and {character:petowner:possPronoun} cat's name is Sniffles.
 Together, it takes you a few hours to find Sniffles. {character:petowner:name:cap} thanks you profusely for your help. Then, you continue on your way to {location:goal:namewiththe}.</t>
   </si>
   <si>
@@ -528,10 +551,10 @@
     <t xml:space="preserve">MF1</t>
   </si>
   <si>
-    <t xml:space="preserve">location:current:baronhome&amp;location:pathtobaron:forest|location:pathtobaron:swamp&amp;goal:hometown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and they begin to chase after you. You sprint into the {location:current:type} as fast as you can.{|SET:chasedbybaron:true|}{|GOTO:pathtobaron|}
+    <t xml:space="preserve">location:current:baronhome&amp;location:pathtobaron:forest&amp;goal:hometown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and they begin to chase after you. You sprint into the {location:pathtobaron:type} as fast as you can.{|SET:chasedbybaron:true|}{|GOTO:pathtobaron|}
 The {character:baron:baron}'s men are chasing you through {location:current:namewiththe} on your way back to {location:goal:name}. If they catch you, there's no telling what they might do to you. To avoid notice, you...{|CRT1|}</t>
   </si>
   <si>
@@ -543,10 +566,10 @@
   <si>
     <t xml:space="preserve">Your nights are uncomfortable. You wake up each morning covered in dirt or leaves or both.
 One night, you're woken in the middle of the night by the sound of men's footsteps. The {character:baron:baron}'s men are searching {location:current:namewiththe} for you. They almost find your hiding spot, but you hear skittering in the trees, and the {character:baron:baron}'s men go off to investigate the sound. You see a flash of red in the trees, possibly two eyes looking at you, and then it's gone.
-You keep going, and you manage to stay ahead of the {character:baron:baron}'s men.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You push on through the night. You're exhausted by the time you reach {location:goal:name}, but you are ahead of the {character:baron:baron}'s men.</t>
+You keep going. Thanks to your mysterious benefactor, you seem to have given the {charac}'s men the slip.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You push on through the night. You're exhausted, but the {character:baron:baron}'s men are nowhere to be seen. You seem to have given them the slip.</t>
   </si>
   <si>
     <t xml:space="preserve">RFW1</t>
@@ -564,8 +587,7 @@
     <t xml:space="preserve">MOTW1</t>
   </si>
   <si>
-    <t xml:space="preserve">You organize a secret meeting at night to rally the people together. You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:current:namewiththe}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they retreat, leaving the town forever.
-The next day, the men who were pursuing you arrive. {location:current:namewiththe:cap}'s finest easily chases them off. There is strength in numbers, and they knew what to expect, thanks to you.{|FTL1|}</t>
+    <t xml:space="preserve">You organize a secret meeting at night to rally the people together. You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:current:namewiththe}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they retreat, leaving the town forever.{|FTL1|}</t>
   </si>
   <si>
     <t xml:space="preserve">FTL1</t>
@@ -863,12 +885,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -970,10 +996,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1098,390 +1124,482 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="1" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="1" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="1" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+    <row r="13" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="1" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>119</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rewriting location replacement to add a "pick" command--it's the only way that a new location can be created or named
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory.Console/Scenes.xlsx
+++ b/Solution/NeverendingStory.Console/Scenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="170">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -49,9 +49,34 @@
     <t xml:space="preserve">location:current:hometown</t>
   </si>
   <si>
-    <t xml:space="preserve">{name}, you live in {location:hometown:name}, a small village {location:hometown:feature:relativeposition}. You work {industry:hometown:workplace} every day, {industry:hometown:goodsGer} enough {industry:hometown:goods} {industry:hometown:purpose} your small village.
-One day, a messenger rides into town. "Citizens of {location:hometown:name}, the {character:antagonist:baron:baron} {character:baron:name} lays claim to your city. You are now under {character:baron:possPronoun} rule and will pay taxes and fealty to {character:baron:objPronoun}."
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{name}, you live in {location:hometown:name}, a small village {location:hometown:feature:relativeposition}. You work {industry:hometown:workplace} every day, {industry:hometown:goodsGer} enough {industry:hometown:goods} {industry:hometown:purpose} your small village.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{location:pick:forest|mountain|swamp|plains:current:pathtobaron}{location:pick:fortress:pathtobaron:baronhome}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">One day, a messenger rides into town. "Citizens of {location:hometown:name}, the {character:antagonist:baron:baron} {character:baron:name} lays claim to your city. You are now under {character:baron:possPronoun} rule and will pay taxes and fealty to {character:baron:objPronoun}."
 What do you do?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Leave {location:hometown:name} to tell the {character:baron:baron} that {character:baron:subPronoun} doesn't own you</t>
@@ -60,8 +85,7 @@
     <t xml:space="preserve">Go to work like always and see if anything changes</t>
   </si>
   <si>
-    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:fortress:namewiththe:baronhome}. You know the way, which leads through the nearby {location:nearby:forest|mountain|swamp|plains:pathtobaron:name}.{|GOTO:pathtobaron|}{|SET:goal:baronhome|}
-Deep in {location:current:namewiththe}, a {character:mentor:sexAge:ranger} emerges from behind the {location:current:covers}. {character:mentor:subPronoun:cap}'s wearing rough clothing.{|MTM|}</t>
+    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:baronhome:namewiththe}. You know the way, which leads through the nearby {location:pathtobaron:name}.{|GOTO:pathtobaron|}{|SET:goal:baronhome|}{|MTM|}</t>
   </si>
   <si>
     <t xml:space="preserve">{industry:hometown:goodday} {|ROC|}</t>
@@ -75,7 +99,7 @@
   <si>
     <t xml:space="preserve">The next week, the {character:baron:baron}'s men arrive. They are soldiers, well-armed and uniformed, with the insignia of the {character:baron:baron} on their jackets.
 They say they're here to collect taxes, but they take so much more than that. They eat food they don't pay for, destroy property that isn't theirs, and leer at young men and women.
-In the morning, your friend {character:bestfriend:name:stolen} is missing. {character:stolen:possPronoun:cap} family says that {character:stolen:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s {location:fortress:name:baronhome} by {character:baron:possPronoun} men. They don't know when, or if, {character:stolen:subPronoun} will return.{|SET:goal:baronhome|}</t>
+In the morning, your friend {character:bestfriend:name:stolen} is missing. {character:stolen:possPronoun:cap} family says that {character:stolen:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s {location:baronhome:name} by {character:baron:possPronoun} men. They don't know when, or if, {character:stolen:subPronoun} will return.{|SET:goal:baronhome|}</t>
   </si>
   <si>
     <t xml:space="preserve">Set out for {location:baronhome:namewiththe} immediately</t>
@@ -84,6 +108,30 @@
     <t xml:space="preserve">Start a fight with the {character:baron:baron}'s men</t>
   </si>
   <si>
+    <t xml:space="preserve">You slink into the nearby {location:pathtobaron:name} in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}
+The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You find a group of the {character:baron:baron}'s men in the tavern drinking. As one of them turns to you, your first blow lands squarely on his jaw. An all-out brawl breaks out. You give as good as you get, but in the end there are too many of them.
+"I'll take care of {objPronoun}," you hear a voice say. Rough hands carry you out of town into the nearby {location:pathtobaron:name}. You pass out.{|GOTO:pathtobaron|}
+You wake up the next day, deep in {location:current:namewiththe}. A {character:mentor:sexAge:ranger} sits under a nearby tree. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?"{|MTM1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTM1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal:baronhome&amp;location:current:forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That day, deep in {location:current:namewiththe}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:ranger:subPronoun:cap}'s wearing rough clothing.{|MTM1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTM1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal:baronhome&amp;location:current:mountain</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -91,15 +139,15 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">You slink into the nearby {location:nearby:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">forest|mountain|swamp|plains</t>
+      <t xml:space="preserve">That day, high in {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">location:current:namewiththe</t>
     </r>
     <r>
       <rPr>
@@ -108,11 +156,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">:pathtobaron:name} in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}
-The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the {location:current:covers}. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
-    </r>
-  </si>
-  <si>
+      <t xml:space="preserve">}, a {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:mentor:sexAge:ranger</t>
+    </r>
     <r>
       <rPr>
         <sz val="10"/>
@@ -120,16 +173,15 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">You find a group of the {character:baron:baron}'s men in the tavern drinking. As one of them turns to you, your first blow lands squarely on his jaw. An all-out brawl breaks out. You give as good as you get, but in the end there are too many of them.
-"I'll take care of {objPronoun}," you hear a voice say. Rough hands carry you out of town into the nearby {location:nearby:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">forest|mountain|swamp|plains</t>
+      <t xml:space="preserve">} emerges from behind a rocky outcrop. {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:ranger:subPronoun:cap</t>
     </r>
     <r>
       <rPr>
@@ -138,15 +190,147 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">:pathtobaron:name}. You pass out.{|GOTO:pathtobaron|}
-You wake up the next day, deep in {location:current:namewiththe}. A {character:mentor:sexAge:ranger} sits under a nearby {location:current:cover}. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">MTM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goal:baronhome&amp;character:ranger</t>
+      <t xml:space="preserve">}'s wearing rough clothing.{|MTM1a|}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">MTM1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal:baronhome&amp;location:current:swamp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">That day, deep in {l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocation:current:namewiththe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}, a {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:mentor:sexAge:ranger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">} emerges from behind the trees, wading through the {location:current:type}. {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:ranger:subPronoun:cap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}'s wearing rough clothing.{|MTM1a|}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">MTM1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal:baronhome&amp;location:current:plains</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">That day, far into {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">location:current:namewiththe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}, you suddenly see a {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:mentor:sexAge:ranger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">} walking among the tall grass, right beside you. {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:ranger:subPronoun:cap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}'s wearing rough clothing.{|MTM1a|}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">MTM1a</t>
   </si>
   <si>
     <t xml:space="preserve">"My name's {character:ranger:name}," {character:ranger:subPronoun} says. "{location:hometown:name}'s not the first village that {character:baron:baron} {character:baron:name}'s taken control of. {character:baron:subPronoun:cap}'ll stop at nothing until the whole region is under {character:baron:possPronoun} control. We can't let that happen.
@@ -164,7 +348,7 @@
 You travel through {location:current:namewiththe} for several days.</t>
   </si>
   <si>
-    <t xml:space="preserve">You walk further into the {location:current:type}, headed for {location:goal:namewiththe}. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
+    <t xml:space="preserve">You walk into the {location:current:type}, headed for {location:goal:namewiththe}. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
 You travel through {location:current:namewiththe} for several days.</t>
   </si>
   <si>
@@ -285,14 +469,14 @@
 "What do we have here?" he says. He grabs you roughly by the shoulder and jerks you to your feet. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
   </si>
   <si>
-    <t xml:space="preserve">You tramp through the underbrush towards the sound of footsteps, getting closer as you hike. Then, through the {location:current:covers}, two dozen of the {character:baron:baron}'s men in uniform emerge.
+    <t xml:space="preserve">You tramp through the underbrush towards the sound of footsteps, getting closer as you hike. Then, through the trees, two dozen of the {character:baron:baron}'s men in uniform emerge.
 One of them grabs you roughly by the shoulder. "What do we have here?" he says. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
   </si>
   <si>
     <t xml:space="preserve">BOTW1a</t>
   </si>
   <si>
-    <t xml:space="preserve">Two more men grab your arms and bind them. You're taken to a camp in the woods an hour away. The {character:baron:baron}'s men tie you to a tree and spend the night drinking and making coarse jokes.
+    <t xml:space="preserve">Two more men grab your arms and bind them. You're taken to a camp in the {location:current:type} an hour away. The {character:baron:baron}'s men tie you to a tree and spend the night drinking and making coarse jokes.
 Most of them have fallen asleep, but there is still one awake, on guard, staring into the fire. He isn't looking directly at you, you could try to escape while he isn't looking. What do you do?</t>
   </si>
   <si>
@@ -494,7 +678,7 @@
     <t xml:space="preserve">Take out one of the guards silently, then sneak inside</t>
   </si>
   <si>
-    <t xml:space="preserve">You have to wait until nightfall to sneak in. The cover of dark covers your movements, and you sneak in through a gap in the patrol you've found.
+    <t xml:space="preserve">You have to wait until nightfall to sneak in. The darkness covers your movements, and you sneak in through a gap in the patrol you've found.
 Inside {location:baronhome:namewiththe}, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
   </si>
   <si>
@@ -508,7 +692,7 @@
     <t xml:space="preserve">goal:baronhome&amp;noitem:map</t>
   </si>
   <si>
-    <t xml:space="preserve">You have to wait until nightfall to sneak in. The cover of dark covers your movements, and you sneak in through a gap in the patrol you've found.
+    <t xml:space="preserve">You have to wait until nightfall to sneak in. The darkness covers your movements, and you sneak in through a gap in the patrol you've found.
 Inside {location:baronhome:namewiththe}, you look around for the treasury. While you're looking, you hear voices.{|AWF1a|}</t>
   </si>
   <si>
@@ -996,10 +1180,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1032,7 +1216,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1078,528 +1262,569 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="1" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="1" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="1" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="1" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="F15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="1" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="B16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="B17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="E19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="1" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="1" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="E21" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="3" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+    <row r="25" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="G25" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="1" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="C26" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B27" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D27" s="1" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B29" s="1" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="B30" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+    <row r="31" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="D31" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F31" s="1" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G31" s="1" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>158</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new industries and new scenes
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory.Console/Scenes.xlsx
+++ b/Solution/NeverendingStory.Console/Scenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="176">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -448,7 +448,7 @@
 You continue on your way to {location:goal:namewiththe}.</t>
   </si>
   <si>
-    <t xml:space="preserve">BOTW1</t>
+    <t xml:space="preserve">BOTW1.1</t>
   </si>
   <si>
     <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:forest</t>
@@ -473,10 +473,32 @@
 One of them grabs you roughly by the shoulder. "What do we have here?" he says. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
   </si>
   <si>
+    <t xml:space="preserve">BOTW1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:swamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your path lies through a fetid {location:current:type}, overgrown with vines. The humidity is stifling and flies swarm everywhere.
+After a day or so, you hear footsteps sloshing along the murky ground. They're getting nearer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide in a nearby bush and wait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You climb into a nearby bush and try to make yourself invisible, then wait. As the footsteps get closer, you see two dozen of the {character:baron:baron}'s armed men tramping through the {location:current:type}.
+You hold your breath, but one of them stumbles just too close to you.
+"What do we have here?" he says. He grabs you roughly by the shoulder and jerks you to your feet. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You pick your way through the {location:current:type} on some of the more solid patches, getting closer to the sound of footsteps. Then, through the trees and vines, two dozen of the {character:baron:baron}'s men in uniform emerge.
+One of them grabs you roughly by the shoulder. "What do we have here?" he says. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOTW1a</t>
   </si>
   <si>
-    <t xml:space="preserve">Two more men grab your arms and bind them. You're taken to a camp in the {location:current:type} an hour away. The {character:baron:baron}'s men tie you to a tree and spend the night drinking and making coarse jokes.
+    <t xml:space="preserve">Two more men grab your arms and bind them. You're taken to a camp on a rise in the {location:current:type} about an hour away. The {character:baron:baron}'s men tie you to a tree and spend the night drinking and making coarse jokes.
 Most of them have fallen asleep, but there is still one awake, on guard, staring into the fire. He isn't looking directly at you, you could try to escape while he isn't looking. What do you do?</t>
   </si>
   <si>
@@ -491,7 +513,7 @@
   </si>
   <si>
     <t xml:space="preserve">You close your eyes and eventually fall into a fitful sleep.
-Hours later you feel someone removing your bonds. It's still night out. You turn to look and see {character:ranger:name}'s face. "Didn't think I'd find YOU when I came to investigate. Stay quiet." {character:ranger:subPronoun:cap} finishes cutting your bonds with {character:ranger:possPronoun} knife, and the two of you slip into the night.
+Hours later you feel someone removing your bonds. It's still night out. You turn to look and see {character:ranger:name}'s face. "Didn't think I'd find YOU when I came to investigate. Stay quiet." {character:ranger:subPronoun:cap} finishes cutting your bonds with {character:ranger:possPronoun} knife, and the two of you slip quietly into the night.
 You travel for a few minutes away from the camp before you realize {character:ranger:name} is gone. The sun begins to rise as you silently make your way toward {location:goal:namewiththe}.</t>
   </si>
   <si>
@@ -1180,10 +1202,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1464,18 +1486,21 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="C15" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="1" t="s">
         <v>77</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>78</v>
@@ -1484,12 +1509,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+    <row r="16" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>81</v>
@@ -1512,319 +1534,342 @@
         <v>86</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="E18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="1" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G21" s="1" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G22" s="1" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F25" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G31" s="1" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>159</v>
+        <v>164</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F35" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G35" s="1" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>169</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding rough Almanac, cleaning up Process code, adding scenes, adding descriptive types to locations
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory.Console/Scenes.xlsx
+++ b/Solution/NeverendingStory.Console/Scenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="188">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -65,18 +65,26 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{location:pick:forest|mountain|swamp|plains:current:pathtobaron}{location:pick:fortress:pathtobaron:baronhome}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">One day, a messenger rides into town. "Citizens of {location:hometown:name}, the {character:antagonist:baron:baron} {character:baron:name} lays claim to your city. You are now under {character:baron:possPronoun} rule and will pay taxes and fealty to {character:baron:objPronoun}."
+      <t xml:space="preserve">{location:pick:forest|mountain|swamp|plains:current:pathtobaron}{location:pick:fortress:pathtobaron:baronhome}{character:pick:baronhome:antagonist:baron}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">One day, a messenger rides into town. "Citizens of {location:hometown:name}, the {almanac:[character-baron-baron] [character-baron-name]:lays claim to [location-hometown-namewiththe]}{character:baron:baron} {character:baron:name} lays claim to your city. You are now under {character:baron:possPronoun} rule and will pay taxes and fealty to {character:baron:objPronoun}."{|SET:baronclaimshometown:true|}
 What do you do?</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{character:pick:current:mentor:ranger}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Leave {location:hometown:name} to tell the {character:baron:baron} that {character:baron:subPronoun} doesn't own you</t>
@@ -85,7 +93,49 @@
     <t xml:space="preserve">Go to work like always and see if anything changes</t>
   </si>
   <si>
-    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:baronhome:namewiththe}. You know the way, which leads through the nearby {location:pathtobaron:name}.{|GOTO:pathtobaron|}{|SET:goal:baronhome|}{|MTM|}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:baronhome:namewiththe}.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{almanac:[location-baronhome-namewiththe]:the home of [character-baron-baron] [character-baron-name]}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> You know the way, which leads through the nearby {location:pathtobaron:name}.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{almanac:[location-pathtobaron-namewiththe-cap]:a [location-pathtobaron-type] that lies near [location-hometown-name]}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{|GOTO:pathtobaron|}{|SET:goal:baronhome|}{|MTM|}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">{industry:hometown:goodday} {|ROC|}</t>
@@ -94,12 +144,70 @@
     <t xml:space="preserve">ROC1</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The next week, the {character:baron:baron}'s men arrive. They are soldiers, well-armed and uniformed, with the insignia of the {character:baron:baron} on their jackets.
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">baronclaimshometown:true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">location:current:hometown</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The next week, the {character:baron:baron}'s men arrive. They are soldiers, well-armed and uniformed, with the insignia of the {character:baron:baron} on their jackets.
 They say they're here to collect taxes, but they take so much more than that. They eat food they don't pay for, destroy property that isn't theirs, and leer at young men and women.
-In the morning, your friend {character:bestfriend:name:stolen} is missing. {character:stolen:possPronoun:cap} family says that {character:stolen:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s {location:baronhome:name} by {character:baron:possPronoun} men. They don't know when, or if, {character:stolen:subPronoun} will return.{|SET:goal:baronhome|}</t>
+In the morning, your friend {character:pick:hometown:friend:taken}{character:taken:name} is missing. {character:taken:possPronoun:cap} family says that {character:taken:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s {location:baronhome:name}{almanac:[location-baronhome-namewiththe]:the home of [character-baron-baron] [character-baron-name]}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{almanac:[character-baron-baron] [character-baron-name]:lives in [location-baronhome-namewiththe]}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> by {character:baron:possPronoun} men. They don't know when, or if, {character:taken:subPronoun} will return.{|SET:goal:baronhome|}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Set out for {location:baronhome:namewiththe} immediately</t>
@@ -108,28 +216,68 @@
     <t xml:space="preserve">Start a fight with the {character:baron:baron}'s men</t>
   </si>
   <si>
-    <t xml:space="preserve">You slink into the nearby {location:pathtobaron:name} in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}
-The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You find a group of the {character:baron:baron}'s men in the tavern drinking. As one of them turns to you, your first blow lands squarely on his jaw. An all-out brawl breaks out. You give as good as you get, but in the end there are too many of them.
-"I'll take care of {objPronoun}," you hear a voice say. Rough hands carry you out of town into the nearby {location:pathtobaron:name}. You pass out.{|GOTO:pathtobaron|}
-You wake up the next day, deep in {location:current:namewiththe}. A {character:mentor:sexAge:ranger} sits under a nearby tree. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?"{|MTM1a|}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You slink into the nearby {location:pathtobaron:name}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{almanac:[location-pathtobaron-namewiththe-cap]:a [location-pathtobaron-type] that lies near [location-hometown-name]}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}
+The next day, deep in the {location:current:type}, a {character:ranger:sexAge} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You find a group of the {character:baron:baron}'s men in the tavern drinking. As one of them turns to you, your first blow lands squarely on his jaw. An all-out brawl breaks out. You give as good as you get, but in the end there are too many of them.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{|SET:baronbarfight:true|}
+"I'll take care of {objPronoun}," you hear a voice say.{|GOTO:pathtobaron|}{|MTM|}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">MTM1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">goal:baronhome&amp;location:current:forest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">That day, deep in {location:current:namewiththe}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:ranger:subPronoun:cap}'s wearing rough clothing.{|MTM1a|}</t>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;goal:baronhome&amp;character:ranger&amp;location:current:forest&amp;baronbarfight:false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That day, deep in {location:current:namewiththe}, a {character:ranger:sexAge} emerges from behind the trees. {character:ranger:subPronoun:cap}'s wearing rough clothing.{|MTM1a|}</t>
   </si>
   <si>
     <t xml:space="preserve">MTM1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">goal:baronhome&amp;location:current:mountain</t>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;goal:baronhome&amp;character:ranger&amp;location:current:mountain&amp;baronbarfight:false</t>
   </si>
   <si>
     <r>
@@ -164,7 +312,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">character:mentor:sexAge:ranger</t>
+      <t xml:space="preserve">character:ranger:sexAge</t>
     </r>
     <r>
       <rPr>
@@ -197,7 +345,7 @@
     <t xml:space="preserve">MTM1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">goal:baronhome&amp;location:current:swamp</t>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;goal:baronhome&amp;character:ranger&amp;location:current:swamp&amp;baronbarfight:false</t>
   </si>
   <si>
     <r>
@@ -232,7 +380,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">character:mentor:sexAge:ranger</t>
+      <t xml:space="preserve">character:ranger:sexAge</t>
     </r>
     <r>
       <rPr>
@@ -265,7 +413,7 @@
     <t xml:space="preserve">MTM1.4</t>
   </si>
   <si>
-    <t xml:space="preserve">goal:baronhome&amp;location:current:plains</t>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;goal:baronhome&amp;character:ranger&amp;location:current:plains&amp;baronbarfight:false</t>
   </si>
   <si>
     <r>
@@ -300,7 +448,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">character:mentor:sexAge:ranger</t>
+      <t xml:space="preserve">character:ranger:sexAge</t>
     </r>
     <r>
       <rPr>
@@ -330,10 +478,50 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">MTM1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;goal:baronhome&amp;character:ranger&amp;location:current:forest&amp;baronbarfight:true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rough hands carry you out of town into the nearby {location:pathtobaron:name}{almanac:[location-pathtobaron-namewiththe-cap]:a [location-pathtobaron-type] that lies near [location-hometown-name]}. You pass out.
+You wake up the next day, deep in {location:current:namewiththe}. A {character:ranger:sexAge} sits under a nearby tree. {character:ranger:subPronoun:cap}'s wearing rough clothing. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?{|MTM1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTM1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;goal:baronhome&amp;character:ranger&amp;location:current:mountain&amp;baronbarfight:true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rough hands carry you out of town to the base of the nearby {location:pathtobaron:name}{almanac:[location-pathtobaron-namewiththe-cap]:a [location-pathtobaron-type] that lies near [location-hometown-name]}. You pass out.
+You wake up the next day, looking up at {location:current:namewiththe}. A {character:ranger:sexAge} sits against a nearby rock. {character:ranger:subPronoun:cap}'s wearing rough clothing. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?{|MTM1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTM1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;goal:baronhome&amp;character:ranger&amp;location:current:swamp&amp;baronbarfight:true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rough hands carry you out of town into the nearby {location:pathtobaron:name}{almanac:[location-pathtobaron-namewiththe-cap]:a [location-pathtobaron-type] that lies near [location-hometown-name]}. You pass out.
+You wake up the next day, deep in {location:current:namewiththe}. A {character:ranger:sexAge} sits under a nearby tree, vines hanging above. {character:ranger:subPronoun:cap}'s wearing rough clothing. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?{|MTM1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTM1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;goal:baronhome&amp;character:ranger&amp;location:current:plains&amp;baronbarfight:true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rough hands carry you out of town into the nearby {location:pathtobaron:namewiththe}{almanac:[location-pathtobaron-namewiththe-cap]:a [location-pathtobaron-type] that lies near [location-hometown-name]}. You pass out.
+You wake up the next day, in {location:current:namewiththe}. A {character:ranger:sexAge} sits in the grass nearby. {character:ranger:subPronoun:cap}'s wearing rough clothing. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?{|MTM1a|}</t>
+  </si>
+  <si>
     <t xml:space="preserve">MTM1a</t>
   </si>
   <si>
-    <t xml:space="preserve">"My name's {character:ranger:name}," {character:ranger:subPronoun} says. "{location:hometown:name}'s not the first village that {character:baron:baron} {character:baron:name}'s taken control of. {character:baron:subPronoun:cap}'ll stop at nothing until the whole region is under {character:baron:possPronoun} control. We can't let that happen.
+    <t xml:space="preserve">"My name's {character:ranger:name},"{almanac:[character-ranger-name]:a mysterious [character-ranger-sexAge] somewhere in [location-current-namewiththe]} {character:ranger:subPronoun} says. "{location:hometown:name}'s not the first village that {character:baron:baron} {character:baron:name}'s taken control of. {character:baron:subPronoun:cap}'ll stop at nothing until the whole region is under {character:baron:possPronoun} control. We can't let that happen.
 "If you want to stop {character:baron:objPronoun} and get back {location:hometown:name}, you'll have to make it to {location:baronhome:namewiththe}."</t>
   </si>
   <si>
@@ -401,7 +589,7 @@
     <t xml:space="preserve">Look for a better place to cross farther up</t>
   </si>
   <si>
-    <t xml:space="preserve"> You step very carefully on each stone. Planting your feet solidly on each stone before stepping to the next one, you make it about halfway across the river. Suddenly, a stone that you were stepping on comes loose, careening down the raging river and taking you along with it.
+    <t xml:space="preserve">You step very carefully on each stone. Planting your feet solidly on each stone before stepping to the next one, you make it about halfway across the river. Suddenly, a stone that you were stepping on comes loose, careening down the raging river and taking you along with it.
 You get several bruises before you’re able to catch yourself, much further downstream, including a nasty bruise on your head. You drag yourself to the other side of the river. You’re sore all over, and can’t move for hours.
 Once you feel almost ready, you climb back up the river’s edge to the path and continue on your way to {location:goal:namewiththe}.</t>
   </si>
@@ -451,7 +639,23 @@
     <t xml:space="preserve">BOTW1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:forest</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:forest</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">The {location:current:type} is dense here, overgrown and difficult to travel through.
@@ -476,7 +680,23 @@
     <t xml:space="preserve">BOTW1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:swamp</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:swamp</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Your path lies through a fetid {location:current:type}, overgrown with vines. The humidity is stifling and flies swarm everywhere.
@@ -522,7 +742,7 @@
   <si>
     <t xml:space="preserve">Your path lies through a thick {location:current:type}, overgrown and difficult to travel through.
 After a day or so, it begins to rain heavily. You take shelter in a nearby cave, making your bed in a small alcove. You go to sleep to wait out the rain.
-When you wake up, you hear someone else moving in the cave. Opening your eyes, you see two enormous bears, sitting between your alcove and the door. It’s still raining outside. They seem to be getting ready to lie down. What do you do?</t>
+When you wake up, you hear something else moving in the cave. Opening your eyes, you see two enormous bears, sitting between your alcove and the door. It’s still raining outside. They seem to be laying down to sleep. What do you do?</t>
   </si>
   <si>
     <t xml:space="preserve">Try to scare them out of the cave so you can leave</t>
@@ -544,7 +764,7 @@
   <si>
     <t xml:space="preserve">The mountain pass is rough here. In many places, you have to climb on all fours to make it over the enormous, jagged rocks.
 After a day or so, it begins to rain heavily. You take shelter in a nearby cave, making your bed in a small alcove. You go to sleep to wait out the rain.
-When you wake up, you hear someone else moving in the cave. Opening your eyes, you see two enormous bears, sitting between your alcove and the door. It’s still raining outside. They seem to be getting ready to lie down. What do you do?</t>
+When you wake up, you hear something else moving in the cave. Opening your eyes, you see two enormous bears, sitting between your alcove and the door. It’s still raining outside. They seem to be laying down to sleep. What do you do?</t>
   </si>
   <si>
     <t xml:space="preserve">ROT1</t>
@@ -575,7 +795,32 @@
     <t xml:space="preserve">location:current:town|location:current:forest|location:current:swamp</t>
   </si>
   <si>
-    <t xml:space="preserve">Late in the day, you hear a voice calling out through the {location:current:type}. You hide immediately, but then realize the voice seems to be that of a young {character:child:sexAge:petowner}. You can see {character:petowner:objPronoun} walking alone, calling out for {character:petowner:possPronoun} cat. What do you do?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{character:pick:current:child:petowner}Late in the day, you hear a voice calling out through the {location:current:type}. You hide immediately, but then realize the voice seems to be that of a young {character:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">petowner</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:sexAge}. You can see {character:petowner:objPronoun} walking alone, calling out for {character:petowner:possPronoun} cat. What do you do?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Reveal yourself and offer to help</t>
@@ -620,7 +865,23 @@
     <t xml:space="preserve">MWG1</t>
   </si>
   <si>
-    <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:forest|location:current:swamp</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:forest|location:current:swamp</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">As the sun sets, you see a small hut ahead of you, nestled between the trees. You pause, considering whether or not to investigate, but before you can decide, a group of men and women dressed like {character:ranger:name} steps out from behind the trees, surrounding you.
@@ -639,10 +900,36 @@
 In the morning, you set off for {location:goal:namewiththe} again.</t>
   </si>
   <si>
-    <t xml:space="preserve">"We're on the same side then! Have you met our friend {character:ranger:name}? {character:ranger:subPronoun:cap}'s out somewhere, fighting against the {character:baron:baron}'s influence."
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"We're on the same side then! Have you met our friend {character:ranger:name}? {character:ranger:subPronoun:cap}'s out somewhere, fighting against the {character:baron:baron}'s influence."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{almanac:[character-ranger-name]:part of a group of resistance fighters}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
 You spend the night with the resistance fighters. The {character:baron:baron}'s men, they tell you, are only working for {character:baron:objPronoun} because {character:baron:subPronoun} pays them handsomely. If you can find a way to stop the {character:baron:baron}'s men from being paid, most of {character:baron:possPronoun} influence over the region will be gone.
 They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from {location:baronhome:namewiththe}, allowing you to get inside more easily.
 In the morning, you set off for {location:goal:namewiththe} again.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">WAT1</t>
@@ -667,28 +954,76 @@
     <t xml:space="preserve">Your stomach growls, but you continue on your way. As your food supply dwindles, your limbs grow weaker.</t>
   </si>
   <si>
-    <t xml:space="preserve">AWF1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goal:baronhome&amp;item:map</t>
+    <t xml:space="preserve">AWF1.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome&amp;item:map</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}.{|AWF1a|}</t>
   </si>
   <si>
-    <t xml:space="preserve">AWF2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goal:baronhome&amp;item:map&amp;character:stolen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}. You look around for any sign of {character:stolen:name}.{|AWF1a|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AWF3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goal:baronhome&amp;character:stolen&amp;noitem:map</t>
+    <t xml:space="preserve">AWF1.2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome&amp;item:map&amp;character:stolen</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}. You look around for any sign of {character:taken:name}.{|AWF1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWF1.3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome&amp;character:stolen&amp;noitem:map</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you look for a way in. There's a patrol of guards circling {location:baronhome:namewiththe}. You think you can find a way in between them, but it would be tough. What do you do?</t>
@@ -701,17 +1036,33 @@
   </si>
   <si>
     <t xml:space="preserve">You have to wait until nightfall to sneak in. The darkness covers your movements, and you sneak in through a gap in the patrol you've found.
-Inside {location:baronhome:namewiththe}, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
+Inside {location:baronhome:namewiththe}, you look around for any sign of {character:taken:name}. While you're looking, you hear voices.{|AWF1a|}</t>
   </si>
   <si>
     <t xml:space="preserve">Jumping out from your hiding place as a guard comes by, you take him out quickly and quietly. You drag the body behind a bush before quickly making your way inside {location:baronhome:namewiththe} in the gap in the patrol.
-Inside {location:baronhome:namewiththe}, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AWF4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goal:baronhome&amp;noitem:map</t>
+Inside {location:baronhome:namewiththe}, you look around for any sign of {character:taken:name}. While you're looking, you hear voices.{|AWF1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWF1.4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome&amp;noitem:map</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">You have to wait until nightfall to sneak in. The darkness covers your movements, and you sneak in through a gap in the patrol you've found.
@@ -733,16 +1084,48 @@
     <t xml:space="preserve">A1</t>
   </si>
   <si>
-    <t xml:space="preserve">character:stolen&amp;location:current:baronhome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You find {character:stolen:name} locked in a dungeon with a bunch of other young people. It seems they've been locked up here for some future purpose of the {character:baron:baron}. You set them all free.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">character:taken&amp;location:current:baronhome</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">You find {character:taken:name} locked in a dungeon with a bunch of other young people. It seems they've been locked up here for some future purpose of the {character:baron:baron}. You set them all free.</t>
   </si>
   <si>
     <t xml:space="preserve">UB1</t>
   </si>
   <si>
-    <t xml:space="preserve">location:current:baronhome</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">location:current:baronhome</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Searching in {location:current:namewiththe}, you finally find the treasury. You take out the lone guard, and go inside. Several heavy chests of gold are inside. You dump them out the window into a lake outside {location:current:namewiththe}. The {character:baron:baron}'s gold is gone.</t>
@@ -757,11 +1140,27 @@
     <t xml:space="preserve">MF1</t>
   </si>
   <si>
-    <t xml:space="preserve">location:current:baronhome&amp;location:pathtobaron:forest&amp;goal:hometown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and they begin to chase after you. You sprint into the {location:pathtobaron:type} as fast as you can.{|SET:chasedbybaron:true|}{|GOTO:pathtobaron|}
-The {character:baron:baron}'s men are chasing you through {location:current:namewiththe} on your way back to {location:goal:name}. If they catch you, there's no telling what they might do to you. To avoid notice, you...{|CRT1|}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">location:current:baronhome&amp;location:pathtobaron:forest&amp;goal:hometown</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and they begin to chase after you. You sprint into the {location:pathtobaron:type} as fast as you can.{|GOTO:pathtobaron|}
+The {character:baron:baron}'s men are chasing you through {location:current:namewiththe} on your way back to {location:goal:name}. If they catch you, there's no telling what they might do to you. To avoid notice, you...</t>
   </si>
   <si>
     <t xml:space="preserve">Spend your nights well-hidden, in a hole or under heavy brush</t>
@@ -772,7 +1171,7 @@
   <si>
     <t xml:space="preserve">Your nights are uncomfortable. You wake up each morning covered in dirt or leaves or both.
 One night, you're woken in the middle of the night by the sound of men's footsteps. The {character:baron:baron}'s men are searching {location:current:namewiththe} for you. They almost find your hiding spot, but you hear skittering in the trees, and the {character:baron:baron}'s men go off to investigate the sound. You see a flash of red in the trees, possibly two eyes looking at you, and then it's gone.
-You keep going. Thanks to your mysterious benefactor, you seem to have given the {charac}'s men the slip.</t>
+You keep going. Thanks to your mysterious benefactor, you seem to have given the {character:baron:baron}'s men the slip.</t>
   </si>
   <si>
     <t xml:space="preserve">You push on through the night. You're exhausted, but the {character:baron:baron}'s men are nowhere to be seen. You seem to have given them the slip.</t>
@@ -784,25 +1183,66 @@
     <t xml:space="preserve">CRT1</t>
   </si>
   <si>
-    <t xml:space="preserve">chasedbybaron:true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{|GOTO:hometown|}You finally return to {location:current:name}. The people have been under the rule of the {character:baron:baron}'s men since you left, who have done nothing but drink and destroy property that isn't theirs. The men pursuing you are close behind, maybe a day or so.{|MOTW1|}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">character:baron</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&amp;baronclaimshometown:true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;goal:hometown</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">{|GOTO:hometown|}You finally return to {location:current:name}. Since you left, the people have been under the rule of the {character:baron:baron}'s men, who have done nothing but drink and destroy property that isn't theirs.</t>
   </si>
   <si>
     <t xml:space="preserve">MOTW1</t>
   </si>
   <si>
-    <t xml:space="preserve">You organize a secret meeting at night to rally the people together. You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:current:namewiththe}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they retreat, leaving the town forever.{|FTL1|}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">location:current:hometown</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">You organize a secret meeting at night to rally the people together. You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:current:namewiththe}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they retreat, leaving the town forever.</t>
   </si>
   <si>
     <t xml:space="preserve">FTL1</t>
   </si>
   <si>
-    <t xml:space="preserve">chasedbybaron:true&amp;location:current:hometown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{location:hometown:namewiththe:cap} is now free! Your fellow citizens are eagerly offering you a position of leadership: they want to make you the {chief} of {location:hometown:namewiththe}. What do you do? {|SET:chasedbybaron:false|}</t>
+    <t xml:space="preserve">{location:hometown:namewiththe:cap} is now free!{|SET:baronclaimshometown:false|} Your fellow citizens are eagerly offering you a position of leadership: they want to make you the {chief} of {location:hometown:namewiththe}. What do you do?</t>
   </si>
   <si>
     <t xml:space="preserve">Go back to your old job, {industry:hometown:workGer}</t>
@@ -1202,15 +1642,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="64.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="11.52"/>
   </cols>
@@ -1238,7 +1679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1702,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1284,7 +1725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1295,7 +1736,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1306,7 +1747,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1317,7 +1758,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -1328,548 +1769,592 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="1" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="10" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="1" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="1" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="1" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="1" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+    <row r="17" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="1" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+    <row r="19" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="E19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+    <row r="20" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="E20" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="1" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="B21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="1" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="B22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F21" s="1" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="D24" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F22" s="1" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F23" s="1" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="D26" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="G26" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F27" s="1" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="1" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="F30" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>152</v>
+      <c r="B31" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>149</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D32" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E32" s="1" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C34" s="1" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C35" s="1" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G36" s="1" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improving help message, adding ultimate boon scenes
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory.Console/Scenes.xlsx
+++ b/Solution/NeverendingStory.Console/Scenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="197">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -595,8 +595,7 @@
   </si>
   <si>
     <t xml:space="preserve">You climb up the rocks along the river's edge until you find an enormous tree trunk lying across the river. It looks as though someone has recently cut it down. You're able to nimbly walk across the log and cross the river.
-Climbing back down, you find the path again and continue on your way to
- {location:goal:namewiththe}.</t>
+Climbing back down, you find the path again and continue on your way to {location:goal:namewiththe}.</t>
   </si>
   <si>
     <t xml:space="preserve">CTT2.1</t>
@@ -1106,7 +1105,7 @@
     <t xml:space="preserve">You find {character:taken:name} locked in a dungeon with a bunch of other young people. It seems they've been locked up here for some future purpose of the {character:baron:baron}. You set them all free.</t>
   </si>
   <si>
-    <t xml:space="preserve">UB1</t>
+    <t xml:space="preserve">UB1.1</t>
   </si>
   <si>
     <r>
@@ -1126,14 +1125,130 @@
       </rPr>
       <t xml:space="preserve">location:current:baronhome</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Searching in {location:current:namewiththe}, you finally find the treasury. You take out the lone guard, and go inside. Several heavy chests of gold are inside. You dump them out the window into a lake outside {location:current:namewiththe}. The {character:baron:baron}'s gold is gone.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&amp;item:map</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Searching in {location:current:namewiththe}, you finally find the treasury. You take out the lone guard, and go inside. Several heavy chests of gold are inside.
+Once the gold is gone, the {character:baron:baron} will have nothing to pay {character:baron:possPronoun} army with, and {character:baron:possPronoun} hold over the region will eventually be gone. What do you do with the chests of gold?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Dump them </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">through</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> the window for the guards outside</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Sneak them outside and make sure no one will find them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propping the heavy chest on the windowsill, you open it and pour the coins out the window. You hear voices below: the guards have noticed, and are fighting over the gold among themselves.
+As you keep pouring, the shouts of joy increase. It sounds like the {character:baron:baron} had recruited men from the poorer villages {character:baron:subPronoun} had conquered, promising them good pay in exchange for their service. Many of the guards below take as much gold as they can and run, returning to their homes and families.
+In a few minutes, the {character:baron:baron}'s gold is gone.
+You take a few gold coins for yourself from the last chest before you dump it. Just a few, not enough to slow you down.{|GIVE:goldcoins:A few gold coins:from the [character-baron-baron]'s treasury chests|}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">It takes hours, but you manage to lug each chest of gold outside of {location:current:namewiththe} through the hidden passage. With no shovel, you can’t bury the chests. You want to make sure no one can ever find the gold again.
+Wading into a nearby lake, you open the chests and dump the gold coins as deep into the lake as you can. The lake will pull them under the muck on the bottom, and no one will ever find them. The {character:baron:baron}'s gold is gone.
+You take a few gold coins for yourself from the last chest before you dump it. Just a few, not enough to slow you down.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{|GIVE:goldcoins:A few gold coins:from the [character-baron-baron]'s treasury chests|}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">UB1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;location:current:baronhome&amp;noitem:map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dump them through the window for the guards outside</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">It takes hours, but you manage to lug each chest of gold outside of {location:current:namewiththe} through openings in the guard patrol. With no shovel, you can’t bury the chests. You want to make sure no one can ever find the gold again.
+Wading into a nearby lake, you open the chests and dump the gold coins as deep into the lake as you can. The lake will pull them under the muck on the bottom, and no one will ever find them. The {character:baron:baron}'s gold is gone.
+You take a few gold coins for yourself from the last chest before you dump it. Just a few, not enough to slow you down.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{|GIVE:goldcoins:A few gold coins:from the [character-baron-baron]'s treasury chests|}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ROR1</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">location:current:baronhome</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">You leave {location:current:namewiththe}.{|SET:goal:hometown|}</t>
   </si>
   <si>
@@ -1159,7 +1274,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and they begin to chase after you. You sprint into the {location:pathtobaron:type} as fast as you can.{|GOTO:pathtobaron|}
+    <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and a few nearby begin to chase after you. You sprint into the {location:pathtobaron:type} as fast as you can.{|GOTO:pathtobaron|}
 The {character:baron:baron}'s men are chasing you through {location:current:namewiththe} on your way back to {location:goal:name}. If they catch you, there's no telling what they might do to you. To avoid notice, you...</t>
   </si>
   <si>
@@ -1642,10 +1757,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2262,7 +2377,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>163</v>
       </c>
@@ -2272,89 +2387,124 @@
       <c r="C34" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D34" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>180</v>
+        <v>185</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding nocharacter condition, not repeating last bit of the story if you look at your inventory or whatever (in the console)
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory.Console/Scenes.xlsx
+++ b/Solution/NeverendingStory.Console/Scenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="213">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -108,7 +108,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{almanac:[location-baronhome-namewiththe]:the home of [character-baron-baron] [character-baron-name]}</t>
+      <t xml:space="preserve">{almanac:[location-baronhome-namewiththe]:the home of [character-baron-baron] [character-baron-name]}{almanac:[character-baron-baron] [character-baron-name]:lives in [location-baronhome-namewiththe]}</t>
     </r>
     <r>
       <rPr>
@@ -240,8 +240,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}
-The next day, deep in the {location:current:type}, a {character:ranger:sexAge} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
+      <t xml:space="preserve"> in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}</t>
     </r>
   </si>
   <si>
@@ -861,6 +860,27 @@
 You climb easily out of the pit. The squirrel is nowhere to be seen.</t>
   </si>
   <si>
+    <t xml:space="preserve">ROT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;character:taken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At night, you wonder how your friend {character:taken:name} is right now. It's been a long time since {character:taken:subPronoun} was taken to {location:baronhome:namewiththe} by the {character:baron:baron}'s men.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worry about how {character:taken:subPronoun}'s doing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to sleep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You stay up staring into the fire wondering whether or not {character:taken:name} is safe. It's late before you fall asleep.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You turn over and do your best to fall asleep. The next morning comes quickly. The sun is rising. You set out for {location:baronhome:namewiththe}, hoping to find {character:taken:name} there.</t>
+  </si>
+  <si>
     <t xml:space="preserve">MWG1</t>
   </si>
   <si>
@@ -971,7 +991,24 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">goal:baronhome&amp;item:map</t>
+      <t xml:space="preserve">goal:baronhome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&amp;nocharacter:taken</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;item:map</t>
     </r>
   </si>
   <si>
@@ -996,7 +1033,24 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">goal:baronhome&amp;item:map&amp;character:stolen</t>
+      <t xml:space="preserve">goal:baronhome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&amp;character:taken</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;item:map</t>
     </r>
   </si>
   <si>
@@ -1021,7 +1075,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">goal:baronhome&amp;character:stolen&amp;noitem:map</t>
+      <t xml:space="preserve">goal:baronhome&amp;character:taken&amp;noitem:map</t>
     </r>
   </si>
   <si>
@@ -1060,7 +1114,24 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">goal:baronhome&amp;noitem:map</t>
+      <t xml:space="preserve">goal:baronhome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&amp;nocharacter:taken</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;noitem:map</t>
     </r>
   </si>
   <si>
@@ -1080,7 +1151,7 @@
 The voices fade away as they turn a corner and are gone.</t>
   </si>
   <si>
-    <t xml:space="preserve">A1</t>
+    <t xml:space="preserve">A1.1</t>
   </si>
   <si>
     <r>
@@ -1102,7 +1173,32 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">You find {character:taken:name} locked in a dungeon with a bunch of other young people. It seems they've been locked up here for some future purpose of the {character:baron:baron}. You set them all free.</t>
+    <t xml:space="preserve">Descending into the dungeon, you find {character:taken:name} locked up with a bunch of other young people. It seems they've been locked up here for some future purpose of the {character:baron:baron}. You set them all free.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1.2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">character:baron&amp;baronclaimshometown:true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;location:current:baronhome</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Descending into the dungeon, you find a bunch of young people locked up there. It seems they've been locked up for some future purpose of the {Baron}. You set them all free.</t>
   </si>
   <si>
     <t xml:space="preserve">UB1.1</t>
@@ -1270,12 +1366,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">location:current:baronhome&amp;location:pathtobaron:forest&amp;goal:hometown</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and a few nearby begin to chase after you. You sprint into the {location:pathtobaron:type} as fast as you can.{|GOTO:pathtobaron|}
-The {character:baron:baron}'s men are chasing you through {location:current:namewiththe} on your way back to {location:goal:name}. If they catch you, there's no telling what they might do to you. To avoid notice, you...</t>
+      <t xml:space="preserve">location:current:baronhome&amp;goal:hometown</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and a few nearby begin to chase after you. You sprint into the {location:pathtobaron:type} as fast as you can.{|GOTO:pathtobaron|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;location:current:baronhome&amp;goal:hometown&amp;location:current:forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The {character:baron:baron}'s men are chasing you through {location:current:namewiththe} on your way back to {location:goal:name}. If they catch you, there's no telling what they might do to you. To avoid notice, you...</t>
   </si>
   <si>
     <t xml:space="preserve">Spend your nights well-hidden, in a hole or under heavy brush</t>
@@ -1292,9 +1396,6 @@
     <t xml:space="preserve">You push on through the night. You're exhausted, but the {character:baron:baron}'s men are nowhere to be seen. You seem to have given them the slip.</t>
   </si>
   <si>
-    <t xml:space="preserve">RFW1</t>
-  </si>
-  <si>
     <t xml:space="preserve">CRT1</t>
   </si>
   <si>
@@ -1351,7 +1452,19 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">You organize a secret meeting at night to rally the people together. You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:current:namewiththe}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they retreat, leaving the town forever.</t>
+    <t xml:space="preserve">You organize a secret meeting at night to rally the people together. They are all ears, ready to hear your plan to rid {location:current:namewiththe} of the {character:baron:baron}’s men. What do you tell them?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drive them out with force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poison their drinks and food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:current:namewiththe}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they all retreat, leaving the town forever.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That night, the {character:baron:baron}’s men carouse and as they always do, demanding food from local businesses they never intend to pay for. But this time, in a coordinated effort by the people of {location:current:namewiththe}, their food and drink is all poisoned. The next morning, not one of the {character:baron:baron}’s men in {location:current:namewiththe} is alive. The people of {location:current:namewiththe} bury them outside of town. They will never bother anyone ever again.</t>
   </si>
   <si>
     <t xml:space="preserve">FTL1</t>
@@ -1757,10 +1870,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2244,11 +2357,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -2267,11 +2380,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -2290,48 +2403,48 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>142</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G30" s="1" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2343,64 +2456,64 @@
         <v>155</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="G34" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>170</v>
       </c>
@@ -2408,103 +2521,158 @@
         <v>171</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D35" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="G35" s="1" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="F37" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>189</v>
+      </c>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>191</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>189</v>
+        <v>197</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>